<commit_message>
import button, data structure const
</commit_message>
<xml_diff>
--- a/Авторизация Роли.xlsx
+++ b/Авторизация Роли.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/react/realan-soft/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF4EDB6-3FCD-6746-B208-897BA6422495}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9DB81B-28DC-1941-8688-B0CBA0F67CE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15920" xr2:uid="{C246618F-535D-6247-814C-7F08D63816A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$H$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>admin</t>
   </si>
@@ -51,23 +54,76 @@
     <t>Покупатели</t>
   </si>
   <si>
-    <t>Склад текущий</t>
-  </si>
-  <si>
     <t>Заказы набор</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>Задачи</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>StockOrders</t>
+  </si>
+  <si>
+    <t>Настройки</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>Магазин</t>
+  </si>
+  <si>
+    <t>Setting/ImportData</t>
+  </si>
+  <si>
+    <t>Кабинет заказчика</t>
+  </si>
+  <si>
+    <t>Инфо</t>
+  </si>
+  <si>
+    <t>Номер</t>
+  </si>
+  <si>
+    <t>CustomerDash</t>
+  </si>
+  <si>
+    <t>Склад</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -79,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,12 +143,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -407,81 +483,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B917C7-798E-154C-BBC8-2B3E0D884F27}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{91AD0788-0191-2144-B9B5-D64F804B4F6A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H10">
+      <sortCondition ref="A1:A10"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>